<commit_message>
hoan thanh lam bai tap ve nha hs
</commit_message>
<xml_diff>
--- a/database/seeders/_khoa_hoc_seeder.xlsx
+++ b/database/seeders/_khoa_hoc_seeder.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="8160" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28725" windowHeight="8160" firstSheet="1" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="khoa_hoc" sheetId="7" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="145" uniqueCount="110">
   <si>
     <t>1) GV phát phiếu học tập.
 - Hãy ghi vào ô chữ Đ trước những hành vi đúng, chữ S trước những hành vi sai (Câu hỏi bài 4 vở bài tập Đạo đức trang 7).
@@ -316,9 +316,6 @@
     <t>Trắc nghiệm</t>
   </si>
   <si>
-    <t>Tự luận</t>
-  </si>
-  <si>
     <t>baitap/1.png</t>
   </si>
   <si>
@@ -382,12 +379,6 @@
     <t>Nhà thờ thánh Basil là công trình của nước nào?</t>
   </si>
   <si>
-    <t>Pháp</t>
-  </si>
-  <si>
-    <t>Nga</t>
-  </si>
-  <si>
     <t>baigiang/bai_giang_1_1.pdf</t>
   </si>
   <si>
@@ -428,6 +419,12 @@
   </si>
   <si>
     <t>anh/khoahoc/belamgame/3.png</t>
+  </si>
+  <si>
+    <t>Các đáp án trên đều sai</t>
+  </si>
+  <si>
+    <t>a</t>
   </si>
 </sst>
 </file>
@@ -475,7 +472,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -491,7 +488,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1087,7 +1083,7 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="B2">
         <v>1</v>
@@ -1095,7 +1091,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
       <c r="B3">
         <v>1</v>
@@ -1103,7 +1099,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>107</v>
+        <v>104</v>
       </c>
       <c r="B4">
         <v>1</v>
@@ -1111,7 +1107,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>108</v>
+        <v>105</v>
       </c>
       <c r="B5">
         <v>2</v>
@@ -1119,7 +1115,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>109</v>
+        <v>106</v>
       </c>
       <c r="B6">
         <v>2</v>
@@ -1127,7 +1123,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>110</v>
+        <v>107</v>
       </c>
       <c r="B7">
         <v>2</v>
@@ -1177,7 +1173,7 @@
         <v>67</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>99</v>
       </c>
       <c r="C2">
         <v>3</v>
@@ -1194,7 +1190,7 @@
         <v>69</v>
       </c>
       <c r="B3" t="s">
-        <v>103</v>
+        <v>100</v>
       </c>
       <c r="C3">
         <v>3</v>
@@ -1211,7 +1207,7 @@
         <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>104</v>
+        <v>101</v>
       </c>
       <c r="C4">
         <v>2</v>
@@ -1232,7 +1228,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+    <sheetView zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
       <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
@@ -1267,7 +1263,7 @@
         <v>8</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="D2" s="3">
         <v>7</v>
@@ -1283,7 +1279,7 @@
         <v>6</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>98</v>
+        <v>95</v>
       </c>
       <c r="D3" s="3">
         <v>7</v>
@@ -1299,7 +1295,7 @@
         <v>4</v>
       </c>
       <c r="C4" s="3" t="s">
-        <v>99</v>
+        <v>96</v>
       </c>
       <c r="D4" s="3">
         <v>7</v>
@@ -1315,7 +1311,7 @@
         <v>2</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="D5" s="3">
         <v>7</v>
@@ -1331,7 +1327,7 @@
         <v>0</v>
       </c>
       <c r="C6" s="3" t="s">
-        <v>101</v>
+        <v>98</v>
       </c>
       <c r="D6" s="3">
         <v>7</v>
@@ -1437,8 +1433,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J6"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1493,23 +1489,25 @@
         <v>72</v>
       </c>
       <c r="C2" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="F2" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="F2" s="4" t="s">
+      <c r="G2" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="G2" s="4" t="s">
+      <c r="H2" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I2" s="4" t="s">
         <v>82</v>
-      </c>
-      <c r="H2" s="4"/>
-      <c r="I2" s="4" t="s">
-        <v>83</v>
       </c>
       <c r="J2" s="4">
         <v>1</v>
@@ -1523,23 +1521,25 @@
         <v>72</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D3" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>84</v>
       </c>
-      <c r="E3" s="8" t="s">
+      <c r="F3" s="4" t="s">
         <v>85</v>
       </c>
-      <c r="F3" s="4" t="s">
+      <c r="G3" s="4" t="s">
         <v>86</v>
       </c>
-      <c r="G3" s="4" t="s">
+      <c r="H3" s="4" t="s">
+        <v>108</v>
+      </c>
+      <c r="I3" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="H3" s="4"/>
-      <c r="I3" s="4" t="s">
-        <v>88</v>
       </c>
       <c r="J3" s="4">
         <v>1</v>
@@ -1553,23 +1553,25 @@
         <v>72</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>76</v>
-      </c>
-      <c r="D4" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>88</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>89</v>
       </c>
-      <c r="E4" s="8" t="s">
+      <c r="F4" s="4" t="s">
         <v>90</v>
       </c>
-      <c r="F4" s="4" t="s">
+      <c r="G4" s="4" t="s">
         <v>91</v>
       </c>
-      <c r="G4" s="4" t="s">
-        <v>92</v>
-      </c>
-      <c r="H4" s="4"/>
+      <c r="H4" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="I4" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="J4" s="4">
         <v>1</v>
@@ -1580,20 +1582,28 @@
         <v>71</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="D5" s="4" t="s">
-        <v>93</v>
-      </c>
-      <c r="E5" s="7"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
+        <v>92</v>
+      </c>
+      <c r="E5" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G5" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H5" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="I5" s="4" t="s">
-        <v>95</v>
+        <v>109</v>
       </c>
       <c r="J5" s="4">
         <v>2</v>
@@ -1604,20 +1614,28 @@
         <v>71</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C6" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D6" s="4" t="s">
-        <v>94</v>
-      </c>
-      <c r="E6" s="8"/>
-      <c r="F6" s="4"/>
-      <c r="G6" s="4"/>
-      <c r="H6" s="4"/>
+        <v>93</v>
+      </c>
+      <c r="E6" s="7" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="4" t="s">
+        <v>108</v>
+      </c>
       <c r="I6" s="4" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="J6" s="4">
         <v>2</v>

</xml_diff>